<commit_message>
HG-304 AEF: Excel and CSV Report genration
</commit_message>
<xml_diff>
--- a/backend/services/libs/shared/src/templates/aef_holdings_template.xlsx
+++ b/backend/services/libs/shared/src/templates/aef_holdings_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmilaDissanayake\Projects\carbon-registry-undp\carbon-registry-zim\backend\services\libs\shared\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB499947-197F-46C4-85CF-EC9F01DBA46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0940FFC5-63D2-4534-9188-86F9166F2B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A6097B3-A9B2-43A8-BF23-64D8708A96D2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A6097B3-A9B2-43A8-BF23-64D8708A96D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Holdings" sheetId="7" r:id="rId1"/>
@@ -39,48 +39,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Article 6 database record ID </t>
   </si>
   <si>
-    <r>
-      <t>Cooperative approach</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
     <t>ITMO</t>
   </si>
   <si>
-    <r>
-      <t>First transfer definition</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-  </si>
-  <si>
     <t>Unique identifier</t>
   </si>
   <si>
@@ -91,105 +57,6 @@
   </si>
   <si>
     <t>Authorization</t>
-  </si>
-  <si>
-    <r>
-      <t>First unique identifier</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Last unique identifier</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>c</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Underlying unit block start ID</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>d</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Underlying unit last block end</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>e</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Metric</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Quantity (expressed in metric)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>g</t>
-    </r>
   </si>
   <si>
     <r>
@@ -220,6 +87,33 @@
     </r>
   </si>
   <si>
+    <t>Purposes for authorization</t>
+  </si>
+  <si>
+    <t>Table3: Holdings</t>
+  </si>
+  <si>
+    <t>Cooperative approach</t>
+  </si>
+  <si>
+    <t>First unique identifier</t>
+  </si>
+  <si>
+    <t>Last unique identifier</t>
+  </si>
+  <si>
+    <t>Underlying unit block start ID</t>
+  </si>
+  <si>
+    <t>Underlying unit last block end</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Quantity (expressed in metric)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Conversion factor </t>
     </r>
@@ -242,560 +136,37 @@
       </rPr>
       <t>(reporting Party)</t>
     </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>h</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>First transferring participating Party</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>i</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Vintage</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>j</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Sector(s)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>k</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Activity type(s)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>l</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Date of authorization</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>m</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Authorization ID</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>n</t>
-    </r>
-  </si>
-  <si>
-    <t>Purposes for authorization</t>
-  </si>
-  <si>
-    <r>
-      <t>OIMP authorized by the Party</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>o</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Name/ID of the cooperative approach as per common nomenclatures.</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> First ITMO unique identifier.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Last ITMO unique identifier. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Underlying unit block end ID for ITMOs recorded on the basis of cooperative approach units tracked in a an underlying cooperative approach registry.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> GHG or non-GHG.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> For non-GHG, the metric in which the ITMO was generated as per common nomenclatures.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> The conversion method or factor of the non-GHG units in the reporting Party’s as per decision 2/CMA.3, annex, para. 22(d).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>j</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Year in which the mitigation outcome occurred.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Sector(s) where the mitigation outcome occurred as per common nomenclatures based on IPCC guidelines.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>l</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Description of the mitigation activity type(s) as per common nomenclatures.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Date of authorization by first transferring Party.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Authorization ID as assigned by the first transferring Party, may include a link to the public evidence of authorization by the first transferring Party.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Fill when “Purposes for authorization” is “OIMP” or “NDC and OIMP”.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> If OIMP is authorized, the first transferring participating Party definition of “first transfer” as per decision 2/CMA.3, annex, para. 2(b).</t>
-    </r>
-  </si>
-  <si>
-    <t>Table3: Holdings</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Underlying unit block start ID for ITMOs recorded on the basis of cooperative approach units tracked in an underlying cooperative approach registry.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Participating Party in which the mitigation outcome was generated as per common nomenclatures.</t>
-    </r>
+  </si>
+  <si>
+    <t>First transferring participating Party</t>
+  </si>
+  <si>
+    <t>Vintage</t>
+  </si>
+  <si>
+    <t>Sector(s)</t>
+  </si>
+  <si>
+    <t>Activity type(s)</t>
+  </si>
+  <si>
+    <t>Date of authorization</t>
+  </si>
+  <si>
+    <t>Authorization ID</t>
+  </si>
+  <si>
+    <t>OIMP authorized by the Party</t>
+  </si>
+  <si>
+    <t>First transfer definition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,14 +176,6 @@
     </font>
     <font>
       <i/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <vertAlign val="superscript"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -868,43 +231,11 @@
     <font>
       <b/>
       <i/>
-      <vertAlign val="superscript"/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
       <vertAlign val="subscript"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <vertAlign val="superscript"/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -991,10 +322,10 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1003,27 +334,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1349,7 +680,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,7 +718,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -1395,10 +726,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>2</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -1416,32 +747,32 @@
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
       <c r="S4" s="12" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
       <c r="O5" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
@@ -1452,49 +783,49 @@
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>23</v>
@@ -1502,84 +833,52 @@
       <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A7" s="6"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A8" s="6"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A9" s="6"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="A17" s="6"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="A19" s="6"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="A20" s="6"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="A22" s="6"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
@@ -1622,12 +921,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f3801cd2-1656-42b6-a361-01c162c981d7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d8fda5c-05ec-4e71-ae39-42f33d20b2eb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1860,20 +1161,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f3801cd2-1656-42b6-a361-01c162c981d7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d8fda5c-05ec-4e71-ae39-42f33d20b2eb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EECD39DE-2373-4013-BB1A-947D9C34A5ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23AE2432-8CDD-42B8-8ACB-9372317A0BFE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f3801cd2-1656-42b6-a361-01c162c981d7"/>
+    <ds:schemaRef ds:uri="6d8fda5c-05ec-4e71-ae39-42f33d20b2eb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1898,12 +1200,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23AE2432-8CDD-42B8-8ACB-9372317A0BFE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EECD39DE-2373-4013-BB1A-947D9C34A5ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f3801cd2-1656-42b6-a361-01c162c981d7"/>
-    <ds:schemaRef ds:uri="6d8fda5c-05ec-4e71-ae39-42f33d20b2eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>